<commit_message>
update bom (added led ring)
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec633e3163aaf01c/Michael/Projekte/Photobooth-HQwebcamTouch/cad-files_public.git/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="11_AD4DB114E441178AC67DF48206D3FDD6683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7D8974B-22A4-4147-93F7-37989DC9817E}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="11_AD4DB114E441178AC67DF48206D3FDD6683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A414AD8B-A461-4C3B-953A-4FAE0294326A}"/>
   <bookViews>
-    <workbookView xWindow="20175" yWindow="1515" windowWidth="25590" windowHeight="16725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1530" windowWidth="25590" windowHeight="16725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Total</t>
   </si>
@@ -90,12 +90,6 @@
     <t>Arducam</t>
   </si>
   <si>
-    <t>64MP camera or 16MP camera would work also</t>
-  </si>
-  <si>
-    <t>64mp autofocus camera</t>
-  </si>
-  <si>
     <t>light system for permanent light</t>
   </si>
   <si>
@@ -142,6 +136,24 @@
   </si>
   <si>
     <t>electronics</t>
+  </si>
+  <si>
+    <t>16mp autofocus camera</t>
+  </si>
+  <si>
+    <t>16MP camera or 64MP camera would work also</t>
+  </si>
+  <si>
+    <t>5V RGB LED Ring WS2812B 12-Bit outer diameter 38mm inner diameter 27mm</t>
+  </si>
+  <si>
+    <t>AZ Delivery</t>
+  </si>
+  <si>
+    <t>4260581553432</t>
+  </si>
+  <si>
+    <t>connectors, wires, …</t>
   </si>
 </sst>
 </file>
@@ -197,11 +209,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -231,8 +247,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C1B3981-F5BB-4421-A10F-8FFAAE2A523E}" name="Tabelle1" displayName="Tabelle1" ref="B3:H20" totalsRowCount="1">
-  <autoFilter ref="B3:H19" xr:uid="{7C1B3981-F5BB-4421-A10F-8FFAAE2A523E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7C1B3981-F5BB-4421-A10F-8FFAAE2A523E}" name="Tabelle1" displayName="Tabelle1" ref="B3:H21" totalsRowCount="1">
+  <autoFilter ref="B3:H20" xr:uid="{7C1B3981-F5BB-4421-A10F-8FFAAE2A523E}"/>
   <tableColumns count="7">
     <tableColumn id="3" xr3:uid="{E93F1550-B7CA-4E59-BA30-8C26949A5ABA}" name="Manufacturer"/>
     <tableColumn id="4" xr3:uid="{6997D9E5-0CEE-44D6-BC57-D6EA7D012C92}" name="Model NO"/>
@@ -512,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H21"/>
+  <dimension ref="B3:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +539,7 @@
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -552,7 +568,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
@@ -561,7 +577,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
@@ -579,8 +595,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -593,12 +610,13 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -611,11 +629,11 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
@@ -639,169 +657,177 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>60</v>
+      </c>
+      <c r="F10" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>60</v>
-      </c>
-      <c r="F9" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>60</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
+      <c r="F14" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
         <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>4</v>
-      </c>
-      <c r="F14" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>4</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2</v>
-      </c>
-      <c r="F15" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>2</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>28</v>
-      </c>
-      <c r="F17" s="1">
-        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
@@ -811,21 +837,21 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1">
         <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
@@ -835,37 +861,62 @@
         <v>0</v>
       </c>
       <c r="E19" s="1">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1">
+        <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
         <v>50</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F20" s="1">
         <f>Tabelle1[[#This Row],[Amount]]*Tabelle1[[#This Row],[Price]]</f>
         <v>0</v>
       </c>
-      <c r="G19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="1">
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
         <f>SUM(Tabelle1[Total])</f>
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="1"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H17" r:id="rId1" xr:uid="{1126008A-EA89-4C62-933E-A22CF503038C}"/>
+    <hyperlink ref="H18" r:id="rId1" xr:uid="{1126008A-EA89-4C62-933E-A22CF503038C}"/>
     <hyperlink ref="H8" r:id="rId2" xr:uid="{1DB23187-C0E7-4B6C-9E73-B95C9BAFD4D0}"/>
-    <hyperlink ref="H18" r:id="rId3" xr:uid="{EEACAAF3-272A-47B1-B01C-F772AECC9205}"/>
-    <hyperlink ref="H9" r:id="rId4" xr:uid="{365932F5-CCEA-4141-B5D2-1B227CA04CD8}"/>
-    <hyperlink ref="H13" r:id="rId5" xr:uid="{42E791E2-2CB9-41A7-AEF4-460B9A746380}"/>
+    <hyperlink ref="H19" r:id="rId3" xr:uid="{EEACAAF3-272A-47B1-B01C-F772AECC9205}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{365932F5-CCEA-4141-B5D2-1B227CA04CD8}"/>
+    <hyperlink ref="H14" r:id="rId5" xr:uid="{42E791E2-2CB9-41A7-AEF4-460B9A746380}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{BB4A073A-6B44-4396-8E4B-0C5BD504217C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="260" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="260" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>